<commit_message>
This seems to work for the most part. Need to check arguments and implement graphing features.
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -574,19 +574,19 @@
         <v>12.01264190673828</v>
       </c>
       <c r="C6" t="n">
-        <v>2.920844475933321</v>
+        <v>2.890185992428072</v>
       </c>
       <c r="D6" t="n">
-        <v>3.50332108551396</v>
+        <v>3.714905814451302</v>
       </c>
       <c r="E6" t="n">
-        <v>0.3651035214814868</v>
+        <v>0.4179997037158225</v>
       </c>
       <c r="F6" t="n">
-        <v>1.629437769201222</v>
+        <v>1.543688107481775</v>
       </c>
       <c r="G6" t="n">
-        <v>1.74575349881511</v>
+        <v>1.72069282810891</v>
       </c>
     </row>
     <row r="7">
@@ -597,19 +597,19 @@
         <v>-41.83860397338867</v>
       </c>
       <c r="C7" t="n">
-        <v>2.659297480106434</v>
+        <v>4.016309467720443</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.8097245042667431</v>
+        <v>0.1300111556989939</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2023071000046448</v>
+        <v>0.4901371972304145</v>
       </c>
       <c r="F7" t="n">
-        <v>1.645171086450825</v>
+        <v>2.049247970961359</v>
       </c>
       <c r="G7" t="n">
-        <v>1.218188589753771</v>
+        <v>1.072177638005135</v>
       </c>
     </row>
     <row r="8">
@@ -620,19 +620,19 @@
         <v>-31.49879264831543</v>
       </c>
       <c r="C8" t="n">
-        <v>2.356016008563889</v>
+        <v>1.450728809180919</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6587158627226681</v>
+        <v>2.918115882885407</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2425954644088348</v>
+        <v>0.6100846378576197</v>
       </c>
       <c r="F8" t="n">
-        <v>1.228150973030189</v>
+        <v>1.229658311504014</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8777762550840216</v>
+        <v>0.8051804048969398</v>
       </c>
     </row>
     <row r="9">
@@ -643,19 +643,19 @@
         <v>18.55722618103027</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.6720430974772955</v>
+        <v>2.362842307729407</v>
       </c>
       <c r="D9" t="n">
-        <v>3.808187847745355</v>
+        <v>5.052065509201971</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1451970944131848</v>
+        <v>1.308846612043794</v>
       </c>
       <c r="F9" t="n">
-        <v>1.408362456742319</v>
+        <v>1.514483439887546</v>
       </c>
       <c r="G9" t="n">
-        <v>1.38042602442851</v>
+        <v>2.156965655612491</v>
       </c>
     </row>
     <row r="10">
@@ -666,19 +666,19 @@
         <v>14.4931812286377</v>
       </c>
       <c r="C10" t="n">
-        <v>1.387983868786141</v>
+        <v>3.600943004536212</v>
       </c>
       <c r="D10" t="n">
-        <v>2.281759681484334</v>
+        <v>4.400904943103417</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.2610187768937071</v>
+        <v>1.404581544613537</v>
       </c>
       <c r="F10" t="n">
-        <v>1.387084963369895</v>
+        <v>1.465089618404473</v>
       </c>
       <c r="G10" t="n">
-        <v>1.641575190993414</v>
+        <v>1.859439426993244</v>
       </c>
     </row>
     <row r="11">
@@ -689,19 +689,19 @@
         <v>35.50856399536133</v>
       </c>
       <c r="C11" t="n">
-        <v>4.273672589567485</v>
+        <v>4.895272577004197</v>
       </c>
       <c r="D11" t="n">
-        <v>5.484468090056484</v>
+        <v>8.380442961710859</v>
       </c>
       <c r="E11" t="n">
-        <v>1.840094280748439</v>
+        <v>4.115704686220278</v>
       </c>
       <c r="F11" t="n">
-        <v>1.489193676687087</v>
+        <v>1.534052611338125</v>
       </c>
       <c r="G11" t="n">
-        <v>1.796488075003597</v>
+        <v>1.807094929033588</v>
       </c>
     </row>
     <row r="12">
@@ -712,19 +712,19 @@
         <v>4.392442226409912</v>
       </c>
       <c r="C12" t="n">
-        <v>2.235732564447486</v>
+        <v>3.556280773819503</v>
       </c>
       <c r="D12" t="n">
-        <v>6.361241609291474</v>
+        <v>6.743409376906882</v>
       </c>
       <c r="E12" t="n">
-        <v>3.606138052060389</v>
+        <v>5.339025292833842</v>
       </c>
       <c r="F12" t="n">
-        <v>1.652571091429816</v>
+        <v>1.761070506569439</v>
       </c>
       <c r="G12" t="n">
-        <v>2.293974906802815</v>
+        <v>2.472289524208387</v>
       </c>
     </row>
     <row r="13">
@@ -735,19 +735,19 @@
         <v>17.10367202758789</v>
       </c>
       <c r="C13" t="n">
-        <v>3.225634172325693</v>
+        <v>6.53482650340761</v>
       </c>
       <c r="D13" t="n">
-        <v>3.397113653820869</v>
+        <v>5.77785891826038</v>
       </c>
       <c r="E13" t="n">
-        <v>3.00071973423478</v>
+        <v>4.168688394382894</v>
       </c>
       <c r="F13" t="n">
-        <v>1.62125614033817</v>
+        <v>1.716797499598147</v>
       </c>
       <c r="G13" t="n">
-        <v>2.383909561241147</v>
+        <v>2.702524820403045</v>
       </c>
     </row>
     <row r="14">
@@ -758,19 +758,19 @@
         <v>28.6794490814209</v>
       </c>
       <c r="C14" t="n">
-        <v>4.233872935525688</v>
+        <v>5.216467899905491</v>
       </c>
       <c r="D14" t="n">
-        <v>7.611732589516219</v>
+        <v>8.147669858029859</v>
       </c>
       <c r="E14" t="n">
-        <v>4.072063794677848</v>
+        <v>5.402905851733751</v>
       </c>
       <c r="F14" t="n">
-        <v>1.7534828537285</v>
+        <v>1.83533289546119</v>
       </c>
       <c r="G14" t="n">
-        <v>2.372833234470688</v>
+        <v>2.604037549316263</v>
       </c>
     </row>
     <row r="15">
@@ -781,19 +781,19 @@
         <v>40.09111404418945</v>
       </c>
       <c r="C15" t="n">
-        <v>4.501937528334725</v>
+        <v>5.161883454294133</v>
       </c>
       <c r="D15" t="n">
-        <v>7.823379951184652</v>
+        <v>8.721037702202484</v>
       </c>
       <c r="E15" t="n">
-        <v>4.501878875949707</v>
+        <v>5.540399034816313</v>
       </c>
       <c r="F15" t="n">
-        <v>1.948100491367711</v>
+        <v>1.990818339451958</v>
       </c>
       <c r="G15" t="n">
-        <v>2.97965742450988</v>
+        <v>2.847442186286497</v>
       </c>
     </row>
     <row r="16">
@@ -804,19 +804,19 @@
         <v>30.21818161010742</v>
       </c>
       <c r="C16" t="n">
-        <v>4.666060466001984</v>
+        <v>5.772280344618859</v>
       </c>
       <c r="D16" t="n">
-        <v>8.235016640234173</v>
+        <v>9.178491449275816</v>
       </c>
       <c r="E16" t="n">
-        <v>4.472835801886164</v>
+        <v>5.483974957733746</v>
       </c>
       <c r="F16" t="n">
-        <v>2.071549268806558</v>
+        <v>1.802887611378982</v>
       </c>
       <c r="G16" t="n">
-        <v>3.668721205996093</v>
+        <v>4.175350867531982</v>
       </c>
     </row>
     <row r="17">
@@ -827,19 +827,19 @@
         <v>-46.79662704467773</v>
       </c>
       <c r="C17" t="n">
-        <v>4.425877292785612</v>
+        <v>4.653627239215556</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9032026041690222</v>
+        <v>1.030705509951482</v>
       </c>
       <c r="E17" t="n">
-        <v>3.759423385034869</v>
+        <v>4.066951309461864</v>
       </c>
       <c r="F17" t="n">
-        <v>2.260981562323539</v>
+        <v>2.195359635464623</v>
       </c>
       <c r="G17" t="n">
-        <v>3.358674458632915</v>
+        <v>4.046325449774004</v>
       </c>
     </row>
     <row r="18">
@@ -850,19 +850,19 @@
         <v>-16.02694511413574</v>
       </c>
       <c r="C18" t="n">
-        <v>4.062454202254666</v>
+        <v>4.531042037695504</v>
       </c>
       <c r="D18" t="n">
-        <v>3.675076561882506</v>
+        <v>5.480827786999743</v>
       </c>
       <c r="E18" t="n">
-        <v>2.786335704896901</v>
+        <v>3.498728062791118</v>
       </c>
       <c r="F18" t="n">
-        <v>2.241176634204947</v>
+        <v>2.282756903655365</v>
       </c>
       <c r="G18" t="n">
-        <v>2.28953085825381</v>
+        <v>2.774640648251451</v>
       </c>
     </row>
     <row r="19">
@@ -873,19 +873,19 @@
         <v>-13.55381965637207</v>
       </c>
       <c r="C19" t="n">
-        <v>4.110657281150679</v>
+        <v>4.761101999744116</v>
       </c>
       <c r="D19" t="n">
-        <v>3.297099956269078</v>
+        <v>4.363343947245058</v>
       </c>
       <c r="E19" t="n">
-        <v>1.047941516128815</v>
+        <v>2.165899987081528</v>
       </c>
       <c r="F19" t="n">
-        <v>2.30947278585226</v>
+        <v>2.396366066936376</v>
       </c>
       <c r="G19" t="n">
-        <v>2.592748903861609</v>
+        <v>2.298267337383058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kind of a working state. Python script needs to reflect MATLAB one more closely. Trying to also update the graph whenever the run button is pressed.
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,21 @@
           <t>cf1_simul</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>grpf_simul</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>vu_simul</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>shortage_simul</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -496,6 +511,15 @@
       <c r="G2" t="n">
         <v>1.981070041656494</v>
       </c>
+      <c r="H2" t="n">
+        <v>-0.5064595937728882</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1.192999362945557</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4.666666507720947</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -519,6 +543,15 @@
       <c r="G3" t="n">
         <v>1.375324249267578</v>
       </c>
+      <c r="H3" t="n">
+        <v>0.2062890231609344</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.165635347366333</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -542,6 +575,15 @@
       <c r="G4" t="n">
         <v>1.609140396118164</v>
       </c>
+      <c r="H4" t="n">
+        <v>-2.330345392227173</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1.221376657485962</v>
+      </c>
+      <c r="J4" t="n">
+        <v>5.666666507720947</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -565,6 +607,15 @@
       <c r="G5" t="n">
         <v>1.644927978515625</v>
       </c>
+      <c r="H5" t="n">
+        <v>-2.08102560043335</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1.20171332359314</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4.666666507720947</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -588,6 +639,15 @@
       <c r="G6" t="n">
         <v>1.72069282810891</v>
       </c>
+      <c r="H6" t="n">
+        <v>-0.2500871419906616</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1.184739232063293</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4.666666507720947</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -611,6 +671,15 @@
       <c r="G7" t="n">
         <v>1.072177638005135</v>
       </c>
+      <c r="H7" t="n">
+        <v>-0.6588118672370911</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.073658347129822</v>
+      </c>
+      <c r="J7" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -634,6 +703,15 @@
       <c r="G8" t="n">
         <v>0.8051804048969398</v>
       </c>
+      <c r="H8" t="n">
+        <v>8.748804092407227</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.2628340423107147</v>
+      </c>
+      <c r="J8" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -657,6 +735,15 @@
       <c r="G9" t="n">
         <v>2.156965655612491</v>
       </c>
+      <c r="H9" t="n">
+        <v>-3.022449254989624</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.4582114815711975</v>
+      </c>
+      <c r="J9" t="n">
+        <v>25.33333396911621</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -680,6 +767,15 @@
       <c r="G10" t="n">
         <v>1.859439426993244</v>
       </c>
+      <c r="H10" t="n">
+        <v>-0.6266276240348816</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.6320492029190063</v>
+      </c>
+      <c r="J10" t="n">
+        <v>9.666666984558105</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -703,6 +799,15 @@
       <c r="G11" t="n">
         <v>1.807094929033588</v>
       </c>
+      <c r="H11" t="n">
+        <v>-3.191989183425903</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.7893379926681519</v>
+      </c>
+      <c r="J11" t="n">
+        <v>11.66666698455811</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -726,6 +831,15 @@
       <c r="G12" t="n">
         <v>2.472289524208387</v>
       </c>
+      <c r="H12" t="n">
+        <v>2.508954286575317</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.009974718093872</v>
+      </c>
+      <c r="J12" t="n">
+        <v>48.33333206176758</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -749,6 +863,15 @@
       <c r="G13" t="n">
         <v>2.702524820403045</v>
       </c>
+      <c r="H13" t="n">
+        <v>1.477425456047058</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1.300251245498657</v>
+      </c>
+      <c r="J13" t="n">
+        <v>22.33333396911621</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -772,6 +895,15 @@
       <c r="G14" t="n">
         <v>2.604037549316263</v>
       </c>
+      <c r="H14" t="n">
+        <v>4.266705513000488</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1.632708787918091</v>
+      </c>
+      <c r="J14" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -795,6 +927,15 @@
       <c r="G15" t="n">
         <v>2.847442186286497</v>
       </c>
+      <c r="H15" t="n">
+        <v>5.85883092880249</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1.84051239490509</v>
+      </c>
+      <c r="J15" t="n">
+        <v>19.66666603088379</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -818,6 +959,15 @@
       <c r="G16" t="n">
         <v>4.175350867531982</v>
       </c>
+      <c r="H16" t="n">
+        <v>5.80972146987915</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1.911138534545898</v>
+      </c>
+      <c r="J16" t="n">
+        <v>32.66666793823242</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -841,6 +991,15 @@
       <c r="G17" t="n">
         <v>4.046325449774004</v>
       </c>
+      <c r="H17" t="n">
+        <v>6.041294574737549</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1.843034982681274</v>
+      </c>
+      <c r="J17" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -864,6 +1023,15 @@
       <c r="G18" t="n">
         <v>2.774640648251451</v>
       </c>
+      <c r="H18" t="n">
+        <v>2.111628532409668</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.825654029846191</v>
+      </c>
+      <c r="J18" t="n">
+        <v>23.66666603088379</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -886,6 +1054,15 @@
       </c>
       <c r="G19" t="n">
         <v>2.298267337383058</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-1.174693703651428</v>
+      </c>
+      <c r="I19" t="n">
+        <v>1.724597811698914</v>
+      </c>
+      <c r="J19" t="n">
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added some graphing functionality. Python script still needs work.
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -625,19 +625,19 @@
         <v>12.01264190673828</v>
       </c>
       <c r="C6" t="n">
-        <v>2.890185992428072</v>
+        <v>2.920844475933321</v>
       </c>
       <c r="D6" t="n">
-        <v>3.714905814451302</v>
+        <v>3.50332108551396</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4179997037158225</v>
+        <v>0.3651035214814868</v>
       </c>
       <c r="F6" t="n">
-        <v>1.543688107481775</v>
+        <v>1.629437769201222</v>
       </c>
       <c r="G6" t="n">
-        <v>1.72069282810891</v>
+        <v>1.74575349881511</v>
       </c>
       <c r="H6" t="n">
         <v>-0.2500871419906616</v>
@@ -657,19 +657,19 @@
         <v>-41.83860397338867</v>
       </c>
       <c r="C7" t="n">
-        <v>4.016309467720443</v>
+        <v>2.659297480106434</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1300111556989939</v>
+        <v>-0.8097245042667431</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4901371972304145</v>
+        <v>0.2023071000046448</v>
       </c>
       <c r="F7" t="n">
-        <v>2.049247970961359</v>
+        <v>1.645171086450825</v>
       </c>
       <c r="G7" t="n">
-        <v>1.072177638005135</v>
+        <v>1.218188589753771</v>
       </c>
       <c r="H7" t="n">
         <v>-0.6588118672370911</v>
@@ -689,19 +689,19 @@
         <v>-31.49879264831543</v>
       </c>
       <c r="C8" t="n">
-        <v>1.450728809180919</v>
+        <v>2.356016008563889</v>
       </c>
       <c r="D8" t="n">
-        <v>2.918115882885407</v>
+        <v>0.6587158627226681</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6100846378576197</v>
+        <v>-0.2425954644088348</v>
       </c>
       <c r="F8" t="n">
-        <v>1.229658311504014</v>
+        <v>1.228150973030189</v>
       </c>
       <c r="G8" t="n">
-        <v>0.8051804048969398</v>
+        <v>0.8777762550840216</v>
       </c>
       <c r="H8" t="n">
         <v>8.748804092407227</v>
@@ -721,19 +721,19 @@
         <v>18.55722618103027</v>
       </c>
       <c r="C9" t="n">
-        <v>2.362842307729407</v>
+        <v>-0.6720430974772955</v>
       </c>
       <c r="D9" t="n">
-        <v>5.052065509201971</v>
+        <v>3.808187847745355</v>
       </c>
       <c r="E9" t="n">
-        <v>1.308846612043794</v>
+        <v>0.1451970944131848</v>
       </c>
       <c r="F9" t="n">
-        <v>1.514483439887546</v>
+        <v>1.408362456742319</v>
       </c>
       <c r="G9" t="n">
-        <v>2.156965655612491</v>
+        <v>1.38042602442851</v>
       </c>
       <c r="H9" t="n">
         <v>-3.022449254989624</v>
@@ -753,19 +753,19 @@
         <v>14.4931812286377</v>
       </c>
       <c r="C10" t="n">
-        <v>3.600943004536212</v>
+        <v>1.387983868786141</v>
       </c>
       <c r="D10" t="n">
-        <v>4.400904943103417</v>
+        <v>2.281759681484334</v>
       </c>
       <c r="E10" t="n">
-        <v>1.404581544613537</v>
+        <v>-0.2610187768937071</v>
       </c>
       <c r="F10" t="n">
-        <v>1.465089618404473</v>
+        <v>1.387084963369895</v>
       </c>
       <c r="G10" t="n">
-        <v>1.859439426993244</v>
+        <v>1.641575190993414</v>
       </c>
       <c r="H10" t="n">
         <v>-0.6266276240348816</v>
@@ -785,19 +785,19 @@
         <v>35.50856399536133</v>
       </c>
       <c r="C11" t="n">
-        <v>4.895272577004197</v>
+        <v>4.273672589567485</v>
       </c>
       <c r="D11" t="n">
-        <v>8.380442961710859</v>
+        <v>5.484468090056484</v>
       </c>
       <c r="E11" t="n">
-        <v>4.115704686220278</v>
+        <v>1.840094280748439</v>
       </c>
       <c r="F11" t="n">
-        <v>1.534052611338125</v>
+        <v>1.489193676687087</v>
       </c>
       <c r="G11" t="n">
-        <v>1.807094929033588</v>
+        <v>1.796488075003597</v>
       </c>
       <c r="H11" t="n">
         <v>-3.191989183425903</v>
@@ -817,19 +817,19 @@
         <v>4.392442226409912</v>
       </c>
       <c r="C12" t="n">
-        <v>3.556280773819503</v>
+        <v>2.235732564447486</v>
       </c>
       <c r="D12" t="n">
-        <v>6.743409376906882</v>
+        <v>6.361241609291474</v>
       </c>
       <c r="E12" t="n">
-        <v>5.339025292833842</v>
+        <v>3.606138052060389</v>
       </c>
       <c r="F12" t="n">
-        <v>1.761070506569439</v>
+        <v>1.652571091429816</v>
       </c>
       <c r="G12" t="n">
-        <v>2.472289524208387</v>
+        <v>2.293974906802815</v>
       </c>
       <c r="H12" t="n">
         <v>2.508954286575317</v>
@@ -849,19 +849,19 @@
         <v>17.10367202758789</v>
       </c>
       <c r="C13" t="n">
-        <v>6.53482650340761</v>
+        <v>3.225634172325693</v>
       </c>
       <c r="D13" t="n">
-        <v>5.77785891826038</v>
+        <v>3.397113653820869</v>
       </c>
       <c r="E13" t="n">
-        <v>4.168688394382894</v>
+        <v>3.00071973423478</v>
       </c>
       <c r="F13" t="n">
-        <v>1.716797499598147</v>
+        <v>1.62125614033817</v>
       </c>
       <c r="G13" t="n">
-        <v>2.702524820403045</v>
+        <v>2.383909561241147</v>
       </c>
       <c r="H13" t="n">
         <v>1.477425456047058</v>
@@ -881,19 +881,19 @@
         <v>28.6794490814209</v>
       </c>
       <c r="C14" t="n">
-        <v>5.216467899905491</v>
+        <v>4.233872935525688</v>
       </c>
       <c r="D14" t="n">
-        <v>8.147669858029859</v>
+        <v>7.611732589516219</v>
       </c>
       <c r="E14" t="n">
-        <v>5.402905851733751</v>
+        <v>4.072063794677848</v>
       </c>
       <c r="F14" t="n">
-        <v>1.83533289546119</v>
+        <v>1.7534828537285</v>
       </c>
       <c r="G14" t="n">
-        <v>2.604037549316263</v>
+        <v>2.372833234470688</v>
       </c>
       <c r="H14" t="n">
         <v>4.266705513000488</v>
@@ -913,19 +913,19 @@
         <v>40.09111404418945</v>
       </c>
       <c r="C15" t="n">
-        <v>5.161883454294133</v>
+        <v>4.501937528334725</v>
       </c>
       <c r="D15" t="n">
-        <v>8.721037702202484</v>
+        <v>7.823379951184652</v>
       </c>
       <c r="E15" t="n">
-        <v>5.540399034816313</v>
+        <v>4.501878875949707</v>
       </c>
       <c r="F15" t="n">
-        <v>1.990818339451958</v>
+        <v>1.948100491367711</v>
       </c>
       <c r="G15" t="n">
-        <v>2.847442186286497</v>
+        <v>2.97965742450988</v>
       </c>
       <c r="H15" t="n">
         <v>5.85883092880249</v>
@@ -945,19 +945,19 @@
         <v>30.21818161010742</v>
       </c>
       <c r="C16" t="n">
-        <v>5.772280344618859</v>
+        <v>4.666060466001984</v>
       </c>
       <c r="D16" t="n">
-        <v>9.178491449275816</v>
+        <v>8.235016640234173</v>
       </c>
       <c r="E16" t="n">
-        <v>5.483974957733746</v>
+        <v>4.472835801886164</v>
       </c>
       <c r="F16" t="n">
-        <v>1.802887611378982</v>
+        <v>2.071549268806558</v>
       </c>
       <c r="G16" t="n">
-        <v>4.175350867531982</v>
+        <v>3.668721205996093</v>
       </c>
       <c r="H16" t="n">
         <v>5.80972146987915</v>
@@ -977,19 +977,19 @@
         <v>-46.79662704467773</v>
       </c>
       <c r="C17" t="n">
-        <v>4.653627239215556</v>
+        <v>4.425877292785612</v>
       </c>
       <c r="D17" t="n">
-        <v>1.030705509951482</v>
+        <v>0.9032026041690222</v>
       </c>
       <c r="E17" t="n">
-        <v>4.066951309461864</v>
+        <v>3.759423385034869</v>
       </c>
       <c r="F17" t="n">
-        <v>2.195359635464623</v>
+        <v>2.260981562323539</v>
       </c>
       <c r="G17" t="n">
-        <v>4.046325449774004</v>
+        <v>3.358674458632915</v>
       </c>
       <c r="H17" t="n">
         <v>6.041294574737549</v>
@@ -1009,19 +1009,19 @@
         <v>-16.02694511413574</v>
       </c>
       <c r="C18" t="n">
-        <v>4.531042037695504</v>
+        <v>4.062454202254666</v>
       </c>
       <c r="D18" t="n">
-        <v>5.480827786999743</v>
+        <v>3.675076561882506</v>
       </c>
       <c r="E18" t="n">
-        <v>3.498728062791118</v>
+        <v>2.786335704896901</v>
       </c>
       <c r="F18" t="n">
-        <v>2.282756903655365</v>
+        <v>2.241176634204947</v>
       </c>
       <c r="G18" t="n">
-        <v>2.774640648251451</v>
+        <v>2.28953085825381</v>
       </c>
       <c r="H18" t="n">
         <v>2.111628532409668</v>
@@ -1041,19 +1041,19 @@
         <v>-13.55381965637207</v>
       </c>
       <c r="C19" t="n">
-        <v>4.761101999744116</v>
+        <v>4.110657281150679</v>
       </c>
       <c r="D19" t="n">
-        <v>4.363343947245058</v>
+        <v>3.297099956269078</v>
       </c>
       <c r="E19" t="n">
-        <v>2.165899987081528</v>
+        <v>1.047941516128815</v>
       </c>
       <c r="F19" t="n">
-        <v>2.396366066936376</v>
+        <v>2.30947278585226</v>
       </c>
       <c r="G19" t="n">
-        <v>2.298267337383058</v>
+        <v>2.592748903861609</v>
       </c>
       <c r="H19" t="n">
         <v>-1.174693703651428</v>

</xml_diff>

<commit_message>
First working version of the website. Additional features still to be added.
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,47 +445,102 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>gw_simul</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>gcpi_simul</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>cf1_simul</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cf10_simul</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>grpe_simul</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>gw_simul</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>gcpi_simul</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>diffcpicf_simul</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>cf10_simul</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cf1_simul</t>
+          <t>grpf_simul</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>grpf_simul</t>
+          <t>vu_simul</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>vu_simul</t>
+          <t>shortage_simul</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>shortage_simul</t>
+          <t>gw_simul_orig</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>gcpi_simul_orig</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>cf1_simul_orig</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>cf10_simul_orig</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>grpe_</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>grpf</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>vu</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>shortage</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>contr_gw</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>contr_gcpi</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>contr_cf1</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>contr_cf10</t>
         </is>
       </c>
     </row>
@@ -494,31 +549,64 @@
         <v>43374</v>
       </c>
       <c r="B2" t="n">
+        <v>2.97620415687561</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9268267154693604</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.981070041656494</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.091349124908447</v>
+      </c>
+      <c r="F2" t="n">
         <v>-21.85605049133301</v>
       </c>
-      <c r="C2" t="n">
+      <c r="G2" t="n">
+        <v>-0.5064595937728882</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.192999362945557</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4.666666507720947</v>
+      </c>
+      <c r="J2" t="n">
         <v>2.97620415687561</v>
       </c>
-      <c r="D2" t="n">
+      <c r="K2" t="n">
         <v>0.9268267154693604</v>
       </c>
-      <c r="E2" t="n">
-        <v>-0.8414778113365173</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="L2" t="n">
+        <v>1.981070041656494</v>
+      </c>
+      <c r="M2" t="n">
         <v>2.091349124908447</v>
       </c>
-      <c r="G2" t="n">
-        <v>1.981070041656494</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="N2" t="n">
+        <v>-21.85605049133301</v>
+      </c>
+      <c r="O2" t="n">
         <v>-0.5064595937728882</v>
       </c>
-      <c r="I2" t="n">
+      <c r="P2" t="n">
         <v>1.192999362945557</v>
       </c>
-      <c r="J2" t="n">
+      <c r="Q2" t="n">
         <v>4.666666507720947</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -526,31 +614,64 @@
         <v>43466</v>
       </c>
       <c r="B3" t="n">
+        <v>2.659780740737915</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.264444351196289</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.375324249267578</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.69207775592804</v>
+      </c>
+      <c r="F3" t="n">
         <v>-1.397886753082275</v>
       </c>
-      <c r="C3" t="n">
+      <c r="G3" t="n">
+        <v>0.2062890231609344</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.165635347366333</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" t="n">
         <v>2.659780740737915</v>
       </c>
-      <c r="D3" t="n">
+      <c r="K3" t="n">
         <v>2.264444351196289</v>
       </c>
-      <c r="E3" t="n">
-        <v>0.147429883480072</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="L3" t="n">
+        <v>1.375324249267578</v>
+      </c>
+      <c r="M3" t="n">
         <v>1.69207775592804</v>
       </c>
-      <c r="G3" t="n">
-        <v>1.375324249267578</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="N3" t="n">
+        <v>-1.397886753082275</v>
+      </c>
+      <c r="O3" t="n">
         <v>0.2062890231609344</v>
       </c>
-      <c r="I3" t="n">
+      <c r="P3" t="n">
         <v>1.165635347366333</v>
       </c>
-      <c r="J3" t="n">
+      <c r="Q3" t="n">
         <v>5</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -558,31 +679,64 @@
         <v>43556</v>
       </c>
       <c r="B4" t="n">
+        <v>2.642211437225342</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.503061532974243</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.609140396118164</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.637053370475769</v>
+      </c>
+      <c r="F4" t="n">
         <v>-4.449340343475342</v>
       </c>
-      <c r="C4" t="n">
+      <c r="G4" t="n">
+        <v>-2.330345392227173</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.221376657485962</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5.666666507720947</v>
+      </c>
+      <c r="J4" t="n">
         <v>2.642211437225342</v>
       </c>
-      <c r="D4" t="n">
+      <c r="K4" t="n">
         <v>1.503061532974243</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.0452277660369873</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="L4" t="n">
+        <v>1.609140396118164</v>
+      </c>
+      <c r="M4" t="n">
         <v>1.637053370475769</v>
       </c>
-      <c r="G4" t="n">
-        <v>1.609140396118164</v>
-      </c>
-      <c r="H4" t="n">
+      <c r="N4" t="n">
+        <v>-4.449340343475342</v>
+      </c>
+      <c r="O4" t="n">
         <v>-2.330345392227173</v>
       </c>
-      <c r="I4" t="n">
+      <c r="P4" t="n">
         <v>1.221376657485962</v>
       </c>
-      <c r="J4" t="n">
+      <c r="Q4" t="n">
         <v>5.666666507720947</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -590,31 +744,64 @@
         <v>43647</v>
       </c>
       <c r="B5" t="n">
+        <v>3.496016502380371</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2.113867282867432</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.644927978515625</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.560448408126831</v>
+      </c>
+      <c r="F5" t="n">
         <v>-2.918939352035522</v>
       </c>
-      <c r="C5" t="n">
+      <c r="G5" t="n">
+        <v>-2.08102560043335</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.20171332359314</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4.666666507720947</v>
+      </c>
+      <c r="J5" t="n">
         <v>3.496016502380371</v>
       </c>
-      <c r="D5" t="n">
+      <c r="K5" t="n">
         <v>2.113867282867432</v>
       </c>
-      <c r="E5" t="n">
-        <v>-0.7079646587371826</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="L5" t="n">
+        <v>1.644927978515625</v>
+      </c>
+      <c r="M5" t="n">
         <v>1.560448408126831</v>
       </c>
-      <c r="G5" t="n">
-        <v>1.644927978515625</v>
-      </c>
-      <c r="H5" t="n">
+      <c r="N5" t="n">
+        <v>-2.918939352035522</v>
+      </c>
+      <c r="O5" t="n">
         <v>-2.08102560043335</v>
       </c>
-      <c r="I5" t="n">
+      <c r="P5" t="n">
         <v>1.20171332359314</v>
       </c>
-      <c r="J5" t="n">
+      <c r="Q5" t="n">
         <v>4.666666507720947</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -622,31 +809,64 @@
         <v>43739</v>
       </c>
       <c r="B6" t="n">
+        <v>2.920844475933321</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.50332108551396</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.643576376937208</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.629437769201222</v>
+      </c>
+      <c r="F6" t="n">
         <v>12.01264190673828</v>
       </c>
-      <c r="C6" t="n">
+      <c r="G6" t="n">
+        <v>-0.2500871419906616</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.184739232063293</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.666666507720947</v>
+      </c>
+      <c r="J6" t="n">
         <v>2.920844475933321</v>
       </c>
-      <c r="D6" t="n">
+      <c r="K6" t="n">
         <v>3.50332108551396</v>
       </c>
-      <c r="E6" t="n">
-        <v>0.3651035214814868</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="L6" t="n">
+        <v>1.643576376937208</v>
+      </c>
+      <c r="M6" t="n">
         <v>1.629437769201222</v>
       </c>
-      <c r="G6" t="n">
-        <v>1.74575349881511</v>
-      </c>
-      <c r="H6" t="n">
+      <c r="N6" t="n">
+        <v>12.01264190673828</v>
+      </c>
+      <c r="O6" t="n">
         <v>-0.2500871419906616</v>
       </c>
-      <c r="I6" t="n">
+      <c r="P6" t="n">
         <v>1.184739232063293</v>
       </c>
-      <c r="J6" t="n">
+      <c r="Q6" t="n">
         <v>4.666666507720947</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -654,31 +874,64 @@
         <v>43831</v>
       </c>
       <c r="B7" t="n">
+        <v>2.62486353443764</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.8224280183251671</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.589685184540286</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.572113170302798</v>
+      </c>
+      <c r="F7" t="n">
         <v>-41.83860397338867</v>
       </c>
-      <c r="C7" t="n">
-        <v>2.659297480106434</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.8097245042667431</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.2023071000046448</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1.645171086450825</v>
-      </c>
       <c r="G7" t="n">
-        <v>1.218188589753771</v>
+        <v>-0.6588118672370911</v>
       </c>
       <c r="H7" t="n">
+        <v>1.073658347129822</v>
+      </c>
+      <c r="I7" t="n">
+        <v>12</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2.62486353443764</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0.8224280183251671</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.589685184540286</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.572113170302798</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-41.83860397338867</v>
+      </c>
+      <c r="O7" t="n">
         <v>-0.6588118672370911</v>
       </c>
-      <c r="I7" t="n">
+      <c r="P7" t="n">
         <v>1.073658347129822</v>
       </c>
-      <c r="J7" t="n">
+      <c r="Q7" t="n">
         <v>12</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -686,31 +939,64 @@
         <v>43922</v>
       </c>
       <c r="B8" t="n">
+        <v>2.478507513310722</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.6973179972408781</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.182006459958566</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.491313139750291</v>
+      </c>
+      <c r="F8" t="n">
         <v>-31.49879264831543</v>
       </c>
-      <c r="C8" t="n">
-        <v>2.356016008563889</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.6587158627226681</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-0.2425954644088348</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1.228150973030189</v>
-      </c>
       <c r="G8" t="n">
-        <v>0.8777762550840216</v>
+        <v>8.748804092407227</v>
       </c>
       <c r="H8" t="n">
+        <v>0.2628340423107147</v>
+      </c>
+      <c r="I8" t="n">
+        <v>14</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2.478507513310722</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6973179972408781</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.182006459958566</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.491313139750291</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-31.49879264831543</v>
+      </c>
+      <c r="O8" t="n">
         <v>8.748804092407227</v>
       </c>
-      <c r="I8" t="n">
+      <c r="P8" t="n">
         <v>0.2628340423107147</v>
       </c>
-      <c r="J8" t="n">
+      <c r="Q8" t="n">
         <v>14</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -718,31 +1004,64 @@
         <v>44013</v>
       </c>
       <c r="B9" t="n">
+        <v>-0.5851866069045748</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.859827423951487</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.549208067845804</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.601297700235178</v>
+      </c>
+      <c r="F9" t="n">
         <v>18.55722618103027</v>
       </c>
-      <c r="C9" t="n">
-        <v>-0.6720430974772955</v>
-      </c>
-      <c r="D9" t="n">
-        <v>3.808187847745355</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.1451970944131848</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1.408362456742319</v>
-      </c>
       <c r="G9" t="n">
-        <v>1.38042602442851</v>
+        <v>-3.022449254989624</v>
       </c>
       <c r="H9" t="n">
+        <v>0.4582114815711975</v>
+      </c>
+      <c r="I9" t="n">
+        <v>25.33333396911621</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-0.5851866069045748</v>
+      </c>
+      <c r="K9" t="n">
+        <v>3.859827423951487</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.549208067845804</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.601297700235178</v>
+      </c>
+      <c r="N9" t="n">
+        <v>18.55722618103027</v>
+      </c>
+      <c r="O9" t="n">
         <v>-3.022449254989624</v>
       </c>
-      <c r="I9" t="n">
+      <c r="P9" t="n">
         <v>0.4582114815711975</v>
       </c>
-      <c r="J9" t="n">
+      <c r="Q9" t="n">
         <v>25.33333396911621</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -750,31 +1069,64 @@
         <v>44105</v>
       </c>
       <c r="B10" t="n">
+        <v>1.532569976950621</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2.359928885994272</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.930538557116238</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.654336769972793</v>
+      </c>
+      <c r="F10" t="n">
         <v>14.4931812286377</v>
       </c>
-      <c r="C10" t="n">
-        <v>1.387983868786141</v>
-      </c>
-      <c r="D10" t="n">
-        <v>2.281759681484334</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-0.2610187768937071</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1.387084963369895</v>
-      </c>
       <c r="G10" t="n">
-        <v>1.641575190993414</v>
+        <v>-0.6266276240348816</v>
       </c>
       <c r="H10" t="n">
+        <v>0.6320492029190063</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9.666666984558105</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1.532569976950621</v>
+      </c>
+      <c r="K10" t="n">
+        <v>2.359928885994272</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1.930538557116238</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1.654336769972793</v>
+      </c>
+      <c r="N10" t="n">
+        <v>14.4931812286377</v>
+      </c>
+      <c r="O10" t="n">
         <v>-0.6266276240348816</v>
       </c>
-      <c r="I10" t="n">
+      <c r="P10" t="n">
         <v>0.6320492029190063</v>
       </c>
-      <c r="J10" t="n">
+      <c r="Q10" t="n">
         <v>9.666666984558105</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -782,31 +1134,64 @@
         <v>44197</v>
       </c>
       <c r="B11" t="n">
+        <v>4.49236174839908</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5.619242251286392</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.045174124597719</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.726261054191536</v>
+      </c>
+      <c r="F11" t="n">
         <v>35.50856399536133</v>
       </c>
-      <c r="C11" t="n">
-        <v>4.273672589567485</v>
-      </c>
-      <c r="D11" t="n">
-        <v>5.484468090056484</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1.840094280748439</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1.489193676687087</v>
-      </c>
       <c r="G11" t="n">
-        <v>1.796488075003597</v>
+        <v>-3.191989183425903</v>
       </c>
       <c r="H11" t="n">
+        <v>0.7893379926681519</v>
+      </c>
+      <c r="I11" t="n">
+        <v>11.66666698455811</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4.49236174839908</v>
+      </c>
+      <c r="K11" t="n">
+        <v>5.619242251286392</v>
+      </c>
+      <c r="L11" t="n">
+        <v>2.045174124597719</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.726261054191536</v>
+      </c>
+      <c r="N11" t="n">
+        <v>35.50856399536133</v>
+      </c>
+      <c r="O11" t="n">
         <v>-3.191989183425903</v>
       </c>
-      <c r="I11" t="n">
+      <c r="P11" t="n">
         <v>0.7893379926681519</v>
       </c>
-      <c r="J11" t="n">
+      <c r="Q11" t="n">
         <v>11.66666698455811</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -814,31 +1199,64 @@
         <v>44287</v>
       </c>
       <c r="B12" t="n">
+        <v>2.426354921777689</v>
+      </c>
+      <c r="C12" t="n">
+        <v>6.511403028606294</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.565404917870143</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.883318937686796</v>
+      </c>
+      <c r="F12" t="n">
         <v>4.392442226409912</v>
       </c>
-      <c r="C12" t="n">
-        <v>2.235732564447486</v>
-      </c>
-      <c r="D12" t="n">
-        <v>6.361241609291474</v>
-      </c>
-      <c r="E12" t="n">
-        <v>3.606138052060389</v>
-      </c>
-      <c r="F12" t="n">
-        <v>1.652571091429816</v>
-      </c>
       <c r="G12" t="n">
-        <v>2.293974906802815</v>
+        <v>2.508954286575317</v>
       </c>
       <c r="H12" t="n">
+        <v>1.009974718093872</v>
+      </c>
+      <c r="I12" t="n">
+        <v>48.33333206176758</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2.426354921777689</v>
+      </c>
+      <c r="K12" t="n">
+        <v>6.511403028606294</v>
+      </c>
+      <c r="L12" t="n">
+        <v>2.565404917870143</v>
+      </c>
+      <c r="M12" t="n">
+        <v>1.883318937686796</v>
+      </c>
+      <c r="N12" t="n">
+        <v>4.392442226409912</v>
+      </c>
+      <c r="O12" t="n">
         <v>2.508954286575317</v>
       </c>
-      <c r="I12" t="n">
+      <c r="P12" t="n">
         <v>1.009974718093872</v>
       </c>
-      <c r="J12" t="n">
+      <c r="Q12" t="n">
         <v>48.33333206176758</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -846,31 +1264,64 @@
         <v>44378</v>
       </c>
       <c r="B13" t="n">
+        <v>3.453365118268367</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.574430157754606</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.617699030388895</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.899968678029008</v>
+      </c>
+      <c r="F13" t="n">
         <v>17.10367202758789</v>
       </c>
-      <c r="C13" t="n">
-        <v>3.225634172325693</v>
-      </c>
-      <c r="D13" t="n">
-        <v>3.397113653820869</v>
-      </c>
-      <c r="E13" t="n">
-        <v>3.00071973423478</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1.62125614033817</v>
-      </c>
       <c r="G13" t="n">
-        <v>2.383909561241147</v>
+        <v>1.477425456047058</v>
       </c>
       <c r="H13" t="n">
+        <v>1.300251245498657</v>
+      </c>
+      <c r="I13" t="n">
+        <v>22.33333396911621</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3.453365118268367</v>
+      </c>
+      <c r="K13" t="n">
+        <v>3.574430157754606</v>
+      </c>
+      <c r="L13" t="n">
+        <v>2.617699030388895</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1.899968678029008</v>
+      </c>
+      <c r="N13" t="n">
+        <v>17.10367202758789</v>
+      </c>
+      <c r="O13" t="n">
         <v>1.477425456047058</v>
       </c>
-      <c r="I13" t="n">
+      <c r="P13" t="n">
         <v>1.300251245498657</v>
       </c>
-      <c r="J13" t="n">
+      <c r="Q13" t="n">
         <v>22.33333396911621</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -878,31 +1329,64 @@
         <v>44470</v>
       </c>
       <c r="B14" t="n">
+        <v>4.457383385483923</v>
+      </c>
+      <c r="C14" t="n">
+        <v>7.812108007885445</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2.603983628082156</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2.003499679048085</v>
+      </c>
+      <c r="F14" t="n">
         <v>28.6794490814209</v>
       </c>
-      <c r="C14" t="n">
-        <v>4.233872935525688</v>
-      </c>
-      <c r="D14" t="n">
-        <v>7.611732589516219</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4.072063794677848</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1.7534828537285</v>
-      </c>
       <c r="G14" t="n">
-        <v>2.372833234470688</v>
+        <v>4.266705513000488</v>
       </c>
       <c r="H14" t="n">
+        <v>1.632708787918091</v>
+      </c>
+      <c r="I14" t="n">
+        <v>22</v>
+      </c>
+      <c r="J14" t="n">
+        <v>4.457383385483923</v>
+      </c>
+      <c r="K14" t="n">
+        <v>7.812108007885445</v>
+      </c>
+      <c r="L14" t="n">
+        <v>2.603983628082156</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2.003499679048085</v>
+      </c>
+      <c r="N14" t="n">
+        <v>28.6794490814209</v>
+      </c>
+      <c r="O14" t="n">
         <v>4.266705513000488</v>
       </c>
-      <c r="I14" t="n">
+      <c r="P14" t="n">
         <v>1.632708787918091</v>
       </c>
-      <c r="J14" t="n">
+      <c r="Q14" t="n">
         <v>22</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -910,31 +1394,64 @@
         <v>44562</v>
       </c>
       <c r="B15" t="n">
+        <v>4.741527240123398</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8.035795149322816</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3.246591233005434</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.200677940063331</v>
+      </c>
+      <c r="F15" t="n">
         <v>40.09111404418945</v>
       </c>
-      <c r="C15" t="n">
-        <v>4.501937528334725</v>
-      </c>
-      <c r="D15" t="n">
-        <v>7.823379951184652</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4.501878875949707</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1.948100491367711</v>
-      </c>
       <c r="G15" t="n">
-        <v>2.97965742450988</v>
+        <v>5.85883092880249</v>
       </c>
       <c r="H15" t="n">
+        <v>1.84051239490509</v>
+      </c>
+      <c r="I15" t="n">
+        <v>19.66666603088379</v>
+      </c>
+      <c r="J15" t="n">
+        <v>4.741527240123398</v>
+      </c>
+      <c r="K15" t="n">
+        <v>8.035795149322816</v>
+      </c>
+      <c r="L15" t="n">
+        <v>3.246591233005434</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2.200677940063331</v>
+      </c>
+      <c r="N15" t="n">
+        <v>40.09111404418945</v>
+      </c>
+      <c r="O15" t="n">
         <v>5.85883092880249</v>
       </c>
-      <c r="I15" t="n">
+      <c r="P15" t="n">
         <v>1.84051239490509</v>
       </c>
-      <c r="J15" t="n">
+      <c r="Q15" t="n">
         <v>19.66666603088379</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -942,31 +1459,64 @@
         <v>44652</v>
       </c>
       <c r="B16" t="n">
+        <v>4.914510101920945</v>
+      </c>
+      <c r="C16" t="n">
+        <v>8.462360184962892</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.518084194922744</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2.324739161053456</v>
+      </c>
+      <c r="F16" t="n">
         <v>30.21818161010742</v>
       </c>
-      <c r="C16" t="n">
-        <v>4.666060466001984</v>
-      </c>
-      <c r="D16" t="n">
-        <v>8.235016640234173</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4.472835801886164</v>
-      </c>
-      <c r="F16" t="n">
-        <v>2.071549268806558</v>
-      </c>
       <c r="G16" t="n">
-        <v>3.668721205996093</v>
+        <v>5.80972146987915</v>
       </c>
       <c r="H16" t="n">
+        <v>1.911138534545898</v>
+      </c>
+      <c r="I16" t="n">
+        <v>32.66666793823242</v>
+      </c>
+      <c r="J16" t="n">
+        <v>4.914510101920945</v>
+      </c>
+      <c r="K16" t="n">
+        <v>8.462360184962892</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3.518084194922744</v>
+      </c>
+      <c r="M16" t="n">
+        <v>2.324739161053456</v>
+      </c>
+      <c r="N16" t="n">
+        <v>30.21818161010742</v>
+      </c>
+      <c r="O16" t="n">
         <v>5.80972146987915</v>
       </c>
-      <c r="I16" t="n">
+      <c r="P16" t="n">
         <v>1.911138534545898</v>
       </c>
-      <c r="J16" t="n">
+      <c r="Q16" t="n">
         <v>32.66666793823242</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -974,31 +1524,64 @@
         <v>44743</v>
       </c>
       <c r="B17" t="n">
+        <v>4.530987644907642</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.086403302456671</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.159679259395985</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2.228979836847881</v>
+      </c>
+      <c r="F17" t="n">
         <v>-46.79662704467773</v>
       </c>
-      <c r="C17" t="n">
-        <v>4.425877292785612</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.9032026041690222</v>
-      </c>
-      <c r="E17" t="n">
-        <v>3.759423385034869</v>
-      </c>
-      <c r="F17" t="n">
-        <v>2.260981562323539</v>
-      </c>
       <c r="G17" t="n">
-        <v>3.358674458632915</v>
+        <v>6.041294574737549</v>
       </c>
       <c r="H17" t="n">
+        <v>1.843034982681274</v>
+      </c>
+      <c r="I17" t="n">
+        <v>18</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4.530987644907642</v>
+      </c>
+      <c r="K17" t="n">
+        <v>1.086403302456671</v>
+      </c>
+      <c r="L17" t="n">
+        <v>3.159679259395985</v>
+      </c>
+      <c r="M17" t="n">
+        <v>2.228979836847881</v>
+      </c>
+      <c r="N17" t="n">
+        <v>-46.79662704467773</v>
+      </c>
+      <c r="O17" t="n">
         <v>6.041294574737549</v>
       </c>
-      <c r="I17" t="n">
+      <c r="P17" t="n">
         <v>1.843034982681274</v>
       </c>
-      <c r="J17" t="n">
+      <c r="Q17" t="n">
         <v>18</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1006,31 +1589,64 @@
         <v>44835</v>
       </c>
       <c r="B18" t="n">
+        <v>4.152352593920312</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3.829086583649435</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.308001588488731</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2.173252283259402</v>
+      </c>
+      <c r="F18" t="n">
         <v>-16.02694511413574</v>
       </c>
-      <c r="C18" t="n">
-        <v>4.062454202254666</v>
-      </c>
-      <c r="D18" t="n">
-        <v>3.675076561882506</v>
-      </c>
-      <c r="E18" t="n">
-        <v>2.786335704896901</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2.241176634204947</v>
-      </c>
       <c r="G18" t="n">
-        <v>2.28953085825381</v>
+        <v>2.111628532409668</v>
       </c>
       <c r="H18" t="n">
+        <v>1.825654029846191</v>
+      </c>
+      <c r="I18" t="n">
+        <v>23.66666603088379</v>
+      </c>
+      <c r="J18" t="n">
+        <v>4.152352593920312</v>
+      </c>
+      <c r="K18" t="n">
+        <v>3.829086583649435</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2.308001588488731</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2.173252283259402</v>
+      </c>
+      <c r="N18" t="n">
+        <v>-16.02694511413574</v>
+      </c>
+      <c r="O18" t="n">
         <v>2.111628532409668</v>
       </c>
-      <c r="I18" t="n">
+      <c r="P18" t="n">
         <v>1.825654029846191</v>
       </c>
-      <c r="J18" t="n">
+      <c r="Q18" t="n">
         <v>23.66666603088379</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>0</v>
+      </c>
+      <c r="U18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1038,31 +1654,64 @@
         <v>44927</v>
       </c>
       <c r="B19" t="n">
+        <v>4.17161561064515</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3.426370195286472</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.578060717518183</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2.255472600394167</v>
+      </c>
+      <c r="F19" t="n">
         <v>-13.55381965637207</v>
       </c>
-      <c r="C19" t="n">
-        <v>4.110657281150679</v>
-      </c>
-      <c r="D19" t="n">
-        <v>3.297099956269078</v>
-      </c>
-      <c r="E19" t="n">
-        <v>1.047941516128815</v>
-      </c>
-      <c r="F19" t="n">
-        <v>2.30947278585226</v>
-      </c>
       <c r="G19" t="n">
-        <v>2.592748903861609</v>
+        <v>-1.174693703651428</v>
       </c>
       <c r="H19" t="n">
+        <v>1.724597811698914</v>
+      </c>
+      <c r="I19" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="J19" t="n">
+        <v>4.17161561064515</v>
+      </c>
+      <c r="K19" t="n">
+        <v>3.426370195286472</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2.578060717518183</v>
+      </c>
+      <c r="M19" t="n">
+        <v>2.255472600394167</v>
+      </c>
+      <c r="N19" t="n">
+        <v>-13.55381965637207</v>
+      </c>
+      <c r="O19" t="n">
         <v>-1.174693703651428</v>
       </c>
-      <c r="I19" t="n">
+      <c r="P19" t="n">
         <v>1.724597811698914</v>
       </c>
-      <c r="J19" t="n">
+      <c r="Q19" t="n">
         <v>21.5</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some API calls
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -809,16 +809,16 @@
         <v>43739</v>
       </c>
       <c r="B6" t="n">
-        <v>2.920844475933321</v>
+        <v>2.890185992428072</v>
       </c>
       <c r="C6" t="n">
-        <v>3.50332108551396</v>
+        <v>3.714905814451302</v>
       </c>
       <c r="D6" t="n">
-        <v>1.643576376937208</v>
+        <v>1.515543661379421</v>
       </c>
       <c r="E6" t="n">
-        <v>1.629437769201222</v>
+        <v>1.543688107481775</v>
       </c>
       <c r="F6" t="n">
         <v>12.01264190673828</v>
@@ -833,16 +833,16 @@
         <v>4.666666507720947</v>
       </c>
       <c r="J6" t="n">
-        <v>2.920844475933321</v>
+        <v>2.890185992428072</v>
       </c>
       <c r="K6" t="n">
-        <v>3.50332108551396</v>
+        <v>3.714905814451302</v>
       </c>
       <c r="L6" t="n">
-        <v>1.643576376937208</v>
+        <v>1.515543661379421</v>
       </c>
       <c r="M6" t="n">
-        <v>1.629437769201222</v>
+        <v>1.543688107481775</v>
       </c>
       <c r="N6" t="n">
         <v>12.01264190673828</v>
@@ -874,16 +874,16 @@
         <v>43831</v>
       </c>
       <c r="B7" t="n">
-        <v>2.62486353443764</v>
+        <v>3.947173685352226</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.8224280183251671</v>
+        <v>0.1045052961119888</v>
       </c>
       <c r="D7" t="n">
-        <v>1.589685184540286</v>
+        <v>1.848995291837182</v>
       </c>
       <c r="E7" t="n">
-        <v>1.572113170302798</v>
+        <v>1.902563758827545</v>
       </c>
       <c r="F7" t="n">
         <v>-41.83860397338867</v>
@@ -898,16 +898,16 @@
         <v>12</v>
       </c>
       <c r="J7" t="n">
-        <v>2.62486353443764</v>
+        <v>3.947173685352226</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.8224280183251671</v>
+        <v>0.1045052961119888</v>
       </c>
       <c r="L7" t="n">
-        <v>1.589685184540286</v>
+        <v>1.848995291837182</v>
       </c>
       <c r="M7" t="n">
-        <v>1.572113170302798</v>
+        <v>1.902563758827545</v>
       </c>
       <c r="N7" t="n">
         <v>-41.83860397338867</v>
@@ -939,16 +939,16 @@
         <v>43922</v>
       </c>
       <c r="B8" t="n">
-        <v>2.478507513310722</v>
+        <v>1.707089712754549</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6973179972408781</v>
+        <v>2.999466478598363</v>
       </c>
       <c r="D8" t="n">
-        <v>1.182006459958566</v>
+        <v>1.446321398849405</v>
       </c>
       <c r="E8" t="n">
-        <v>1.491313139750291</v>
+        <v>1.780148400507346</v>
       </c>
       <c r="F8" t="n">
         <v>-31.49879264831543</v>
@@ -963,16 +963,16 @@
         <v>14</v>
       </c>
       <c r="J8" t="n">
-        <v>2.478507513310722</v>
+        <v>1.707089712754549</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6973179972408781</v>
+        <v>2.999466478598363</v>
       </c>
       <c r="L8" t="n">
-        <v>1.182006459958566</v>
+        <v>1.446321398849405</v>
       </c>
       <c r="M8" t="n">
-        <v>1.491313139750291</v>
+        <v>1.780148400507346</v>
       </c>
       <c r="N8" t="n">
         <v>-31.49879264831543</v>
@@ -1004,16 +1004,16 @@
         <v>44013</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.5851866069045748</v>
+        <v>2.548265390879449</v>
       </c>
       <c r="C9" t="n">
-        <v>3.859827423951487</v>
+        <v>5.161811764402577</v>
       </c>
       <c r="D9" t="n">
-        <v>1.549208067845804</v>
+        <v>2.571210205683845</v>
       </c>
       <c r="E9" t="n">
-        <v>1.601297700235178</v>
+        <v>1.924275155794865</v>
       </c>
       <c r="F9" t="n">
         <v>18.55722618103027</v>
@@ -1028,16 +1028,16 @@
         <v>25.33333396911621</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.5851866069045748</v>
+        <v>2.548265390879449</v>
       </c>
       <c r="K9" t="n">
-        <v>3.859827423951487</v>
+        <v>5.161811764402577</v>
       </c>
       <c r="L9" t="n">
-        <v>1.549208067845804</v>
+        <v>2.571210205683845</v>
       </c>
       <c r="M9" t="n">
-        <v>1.601297700235178</v>
+        <v>1.924275155794865</v>
       </c>
       <c r="N9" t="n">
         <v>18.55722618103027</v>
@@ -1069,16 +1069,16 @@
         <v>44105</v>
       </c>
       <c r="B10" t="n">
-        <v>1.532569976950621</v>
+        <v>3.925161465394415</v>
       </c>
       <c r="C10" t="n">
-        <v>2.359928885994272</v>
+        <v>4.573639312412173</v>
       </c>
       <c r="D10" t="n">
-        <v>1.930538557116238</v>
+        <v>2.640929391352556</v>
       </c>
       <c r="E10" t="n">
-        <v>1.654336769972793</v>
+        <v>2.066447829538879</v>
       </c>
       <c r="F10" t="n">
         <v>14.4931812286377</v>
@@ -1093,16 +1093,16 @@
         <v>9.666666984558105</v>
       </c>
       <c r="J10" t="n">
-        <v>1.532569976950621</v>
+        <v>3.925161465394415</v>
       </c>
       <c r="K10" t="n">
-        <v>2.359928885994272</v>
+        <v>4.573639312412173</v>
       </c>
       <c r="L10" t="n">
-        <v>1.930538557116238</v>
+        <v>2.640929391352556</v>
       </c>
       <c r="M10" t="n">
-        <v>1.654336769972793</v>
+        <v>2.066447829538879</v>
       </c>
       <c r="N10" t="n">
         <v>14.4931812286377</v>
@@ -1134,16 +1134,16 @@
         <v>44197</v>
       </c>
       <c r="B11" t="n">
-        <v>4.49236174839908</v>
+        <v>5.41570914763265</v>
       </c>
       <c r="C11" t="n">
-        <v>5.619242251286392</v>
+        <v>8.690423321004072</v>
       </c>
       <c r="D11" t="n">
-        <v>2.045174124597719</v>
+        <v>2.52100251750318</v>
       </c>
       <c r="E11" t="n">
-        <v>1.726261054191536</v>
+        <v>2.160514947755103</v>
       </c>
       <c r="F11" t="n">
         <v>35.50856399536133</v>
@@ -1158,16 +1158,16 @@
         <v>11.66666698455811</v>
       </c>
       <c r="J11" t="n">
-        <v>4.49236174839908</v>
+        <v>5.41570914763265</v>
       </c>
       <c r="K11" t="n">
-        <v>5.619242251286392</v>
+        <v>8.690423321004072</v>
       </c>
       <c r="L11" t="n">
-        <v>2.045174124597719</v>
+        <v>2.52100251750318</v>
       </c>
       <c r="M11" t="n">
-        <v>1.726261054191536</v>
+        <v>2.160514947755103</v>
       </c>
       <c r="N11" t="n">
         <v>35.50856399536133</v>
@@ -1199,16 +1199,16 @@
         <v>44287</v>
       </c>
       <c r="B12" t="n">
-        <v>2.426354921777689</v>
+        <v>4.041327098464382</v>
       </c>
       <c r="C12" t="n">
-        <v>6.511403028606294</v>
+        <v>7.104535720346792</v>
       </c>
       <c r="D12" t="n">
-        <v>2.565404917870143</v>
+        <v>3.246296339093778</v>
       </c>
       <c r="E12" t="n">
-        <v>1.883318937686796</v>
+        <v>2.405517533039561</v>
       </c>
       <c r="F12" t="n">
         <v>4.392442226409912</v>
@@ -1223,16 +1223,16 @@
         <v>48.33333206176758</v>
       </c>
       <c r="J12" t="n">
-        <v>2.426354921777689</v>
+        <v>4.041327098464382</v>
       </c>
       <c r="K12" t="n">
-        <v>6.511403028606294</v>
+        <v>7.104535720346792</v>
       </c>
       <c r="L12" t="n">
-        <v>2.565404917870143</v>
+        <v>3.246296339093778</v>
       </c>
       <c r="M12" t="n">
-        <v>1.883318937686796</v>
+        <v>2.405517533039561</v>
       </c>
       <c r="N12" t="n">
         <v>4.392442226409912</v>
@@ -1264,16 +1264,16 @@
         <v>44378</v>
       </c>
       <c r="B13" t="n">
-        <v>3.453365118268367</v>
+        <v>7.138470407773682</v>
       </c>
       <c r="C13" t="n">
-        <v>3.574430157754606</v>
+        <v>6.223102706575908</v>
       </c>
       <c r="D13" t="n">
-        <v>2.617699030388895</v>
+        <v>3.547903824342392</v>
       </c>
       <c r="E13" t="n">
-        <v>1.899968678029008</v>
+        <v>2.500935234204537</v>
       </c>
       <c r="F13" t="n">
         <v>17.10367202758789</v>
@@ -1288,16 +1288,16 @@
         <v>22.33333396911621</v>
       </c>
       <c r="J13" t="n">
-        <v>3.453365118268367</v>
+        <v>7.138470407773682</v>
       </c>
       <c r="K13" t="n">
-        <v>3.574430157754606</v>
+        <v>6.223102706575908</v>
       </c>
       <c r="L13" t="n">
-        <v>2.617699030388895</v>
+        <v>3.547903824342392</v>
       </c>
       <c r="M13" t="n">
-        <v>1.899968678029008</v>
+        <v>2.500935234204537</v>
       </c>
       <c r="N13" t="n">
         <v>17.10367202758789</v>
@@ -1329,16 +1329,16 @@
         <v>44470</v>
       </c>
       <c r="B14" t="n">
-        <v>4.457383385483923</v>
+        <v>5.88510388946956</v>
       </c>
       <c r="C14" t="n">
-        <v>7.812108007885445</v>
+        <v>8.686755909100066</v>
       </c>
       <c r="D14" t="n">
-        <v>2.603983628082156</v>
+        <v>3.501288734535368</v>
       </c>
       <c r="E14" t="n">
-        <v>2.003499679048085</v>
+        <v>2.657655480666553</v>
       </c>
       <c r="F14" t="n">
         <v>28.6794490814209</v>
@@ -1353,16 +1353,16 @@
         <v>22</v>
       </c>
       <c r="J14" t="n">
-        <v>4.457383385483923</v>
+        <v>5.88510388946956</v>
       </c>
       <c r="K14" t="n">
-        <v>7.812108007885445</v>
+        <v>8.686755909100066</v>
       </c>
       <c r="L14" t="n">
-        <v>2.603983628082156</v>
+        <v>3.501288734535368</v>
       </c>
       <c r="M14" t="n">
-        <v>2.003499679048085</v>
+        <v>2.657655480666553</v>
       </c>
       <c r="N14" t="n">
         <v>28.6794490814209</v>
@@ -1394,16 +1394,16 @@
         <v>44562</v>
       </c>
       <c r="B15" t="n">
-        <v>4.741527240123398</v>
+        <v>5.903278497842052</v>
       </c>
       <c r="C15" t="n">
-        <v>8.035795149322816</v>
+        <v>9.326031465330262</v>
       </c>
       <c r="D15" t="n">
-        <v>3.246591233005434</v>
+        <v>3.788507206940825</v>
       </c>
       <c r="E15" t="n">
-        <v>2.200677940063331</v>
+        <v>2.875771655760958</v>
       </c>
       <c r="F15" t="n">
         <v>40.09111404418945</v>
@@ -1418,16 +1418,16 @@
         <v>19.66666603088379</v>
       </c>
       <c r="J15" t="n">
-        <v>4.741527240123398</v>
+        <v>5.903278497842052</v>
       </c>
       <c r="K15" t="n">
-        <v>8.035795149322816</v>
+        <v>9.326031465330262</v>
       </c>
       <c r="L15" t="n">
-        <v>3.246591233005434</v>
+        <v>3.788507206940825</v>
       </c>
       <c r="M15" t="n">
-        <v>2.200677940063331</v>
+        <v>2.875771655760958</v>
       </c>
       <c r="N15" t="n">
         <v>40.09111404418945</v>
@@ -1459,16 +1459,16 @@
         <v>44652</v>
       </c>
       <c r="B16" t="n">
-        <v>4.914510101920945</v>
+        <v>6.572391498800909</v>
       </c>
       <c r="C16" t="n">
-        <v>8.462360184962892</v>
+        <v>9.855668632346275</v>
       </c>
       <c r="D16" t="n">
-        <v>3.518084194922744</v>
+        <v>4.349832790633939</v>
       </c>
       <c r="E16" t="n">
-        <v>2.324739161053456</v>
+        <v>2.717981976982983</v>
       </c>
       <c r="F16" t="n">
         <v>30.21818161010742</v>
@@ -1483,16 +1483,16 @@
         <v>32.66666793823242</v>
       </c>
       <c r="J16" t="n">
-        <v>4.914510101920945</v>
+        <v>6.572391498800909</v>
       </c>
       <c r="K16" t="n">
-        <v>8.462360184962892</v>
+        <v>9.855668632346275</v>
       </c>
       <c r="L16" t="n">
-        <v>3.518084194922744</v>
+        <v>4.349832790633939</v>
       </c>
       <c r="M16" t="n">
-        <v>2.324739161053456</v>
+        <v>2.717981976982983</v>
       </c>
       <c r="N16" t="n">
         <v>30.21818161010742</v>
@@ -1524,16 +1524,16 @@
         <v>44743</v>
       </c>
       <c r="B17" t="n">
-        <v>4.530987644907642</v>
+        <v>5.231883391341852</v>
       </c>
       <c r="C17" t="n">
-        <v>1.086403302456671</v>
+        <v>1.673691006414161</v>
       </c>
       <c r="D17" t="n">
-        <v>3.159679259395985</v>
+        <v>4.165709660639497</v>
       </c>
       <c r="E17" t="n">
-        <v>2.228979836847881</v>
+        <v>2.591637474714854</v>
       </c>
       <c r="F17" t="n">
         <v>-46.79662704467773</v>
@@ -1548,16 +1548,16 @@
         <v>18</v>
       </c>
       <c r="J17" t="n">
-        <v>4.530987644907642</v>
+        <v>5.231883391341852</v>
       </c>
       <c r="K17" t="n">
-        <v>1.086403302456671</v>
+        <v>1.673691006414161</v>
       </c>
       <c r="L17" t="n">
-        <v>3.159679259395985</v>
+        <v>4.165709660639497</v>
       </c>
       <c r="M17" t="n">
-        <v>2.228979836847881</v>
+        <v>2.591637474714854</v>
       </c>
       <c r="N17" t="n">
         <v>-46.79662704467773</v>
@@ -1589,16 +1589,16 @@
         <v>44835</v>
       </c>
       <c r="B18" t="n">
-        <v>4.152352593920312</v>
+        <v>5.112999863523385</v>
       </c>
       <c r="C18" t="n">
-        <v>3.829086583649435</v>
+        <v>6.10984356365371</v>
       </c>
       <c r="D18" t="n">
-        <v>2.308001588488731</v>
+        <v>3.304065659169891</v>
       </c>
       <c r="E18" t="n">
-        <v>2.173252283259402</v>
+        <v>2.632003991546259</v>
       </c>
       <c r="F18" t="n">
         <v>-16.02694511413574</v>
@@ -1613,16 +1613,16 @@
         <v>23.66666603088379</v>
       </c>
       <c r="J18" t="n">
-        <v>4.152352593920312</v>
+        <v>5.112999863523385</v>
       </c>
       <c r="K18" t="n">
-        <v>3.829086583649435</v>
+        <v>6.10984356365371</v>
       </c>
       <c r="L18" t="n">
-        <v>2.308001588488731</v>
+        <v>3.304065659169891</v>
       </c>
       <c r="M18" t="n">
-        <v>2.173252283259402</v>
+        <v>2.632003991546259</v>
       </c>
       <c r="N18" t="n">
         <v>-16.02694511413574</v>
@@ -1654,16 +1654,16 @@
         <v>44927</v>
       </c>
       <c r="B19" t="n">
-        <v>4.17161561064515</v>
+        <v>5.307787499498914</v>
       </c>
       <c r="C19" t="n">
-        <v>3.426370195286472</v>
+        <v>4.979445338340163</v>
       </c>
       <c r="D19" t="n">
-        <v>2.578060717518183</v>
+        <v>2.790295248693076</v>
       </c>
       <c r="E19" t="n">
-        <v>2.255472600394167</v>
+        <v>2.786496694332275</v>
       </c>
       <c r="F19" t="n">
         <v>-13.55381965637207</v>
@@ -1678,16 +1678,16 @@
         <v>21.5</v>
       </c>
       <c r="J19" t="n">
-        <v>4.17161561064515</v>
+        <v>5.307787499498914</v>
       </c>
       <c r="K19" t="n">
-        <v>3.426370195286472</v>
+        <v>4.979445338340163</v>
       </c>
       <c r="L19" t="n">
-        <v>2.578060717518183</v>
+        <v>2.790295248693076</v>
       </c>
       <c r="M19" t="n">
-        <v>2.255472600394167</v>
+        <v>2.786496694332275</v>
       </c>
       <c r="N19" t="n">
         <v>-13.55381965637207</v>

</xml_diff>

<commit_message>
added some additional console.log functions for testing
</commit_message>
<xml_diff>
--- a/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
+++ b/server/econ_model/data/output_data/dynamic_simul_results_weblab.xlsx
@@ -809,16 +809,16 @@
         <v>43739</v>
       </c>
       <c r="B6" t="n">
-        <v>2.890185992428072</v>
+        <v>2.920844475933321</v>
       </c>
       <c r="C6" t="n">
-        <v>3.714905814451302</v>
+        <v>3.50332108551396</v>
       </c>
       <c r="D6" t="n">
-        <v>1.515543661379421</v>
+        <v>1.643576376937208</v>
       </c>
       <c r="E6" t="n">
-        <v>1.543688107481775</v>
+        <v>1.629437769201222</v>
       </c>
       <c r="F6" t="n">
         <v>12.01264190673828</v>
@@ -833,16 +833,16 @@
         <v>4.666666507720947</v>
       </c>
       <c r="J6" t="n">
-        <v>2.890185992428072</v>
+        <v>2.920844475933321</v>
       </c>
       <c r="K6" t="n">
-        <v>3.714905814451302</v>
+        <v>3.50332108551396</v>
       </c>
       <c r="L6" t="n">
-        <v>1.515543661379421</v>
+        <v>1.643576376937208</v>
       </c>
       <c r="M6" t="n">
-        <v>1.543688107481775</v>
+        <v>1.629437769201222</v>
       </c>
       <c r="N6" t="n">
         <v>12.01264190673828</v>
@@ -874,16 +874,16 @@
         <v>43831</v>
       </c>
       <c r="B7" t="n">
-        <v>3.947173685352226</v>
+        <v>2.62486353443764</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1045052961119888</v>
+        <v>-0.8224280183251671</v>
       </c>
       <c r="D7" t="n">
-        <v>1.848995291837182</v>
+        <v>1.589685184540286</v>
       </c>
       <c r="E7" t="n">
-        <v>1.902563758827545</v>
+        <v>1.572113170302798</v>
       </c>
       <c r="F7" t="n">
         <v>-41.83860397338867</v>
@@ -898,16 +898,16 @@
         <v>12</v>
       </c>
       <c r="J7" t="n">
-        <v>3.947173685352226</v>
+        <v>2.62486353443764</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1045052961119888</v>
+        <v>-0.8224280183251671</v>
       </c>
       <c r="L7" t="n">
-        <v>1.848995291837182</v>
+        <v>1.589685184540286</v>
       </c>
       <c r="M7" t="n">
-        <v>1.902563758827545</v>
+        <v>1.572113170302798</v>
       </c>
       <c r="N7" t="n">
         <v>-41.83860397338867</v>
@@ -939,16 +939,16 @@
         <v>43922</v>
       </c>
       <c r="B8" t="n">
-        <v>1.707089712754549</v>
+        <v>2.478507513310722</v>
       </c>
       <c r="C8" t="n">
-        <v>2.999466478598363</v>
+        <v>0.6973179972408781</v>
       </c>
       <c r="D8" t="n">
-        <v>1.446321398849405</v>
+        <v>1.182006459958566</v>
       </c>
       <c r="E8" t="n">
-        <v>1.780148400507346</v>
+        <v>1.491313139750291</v>
       </c>
       <c r="F8" t="n">
         <v>-31.49879264831543</v>
@@ -963,16 +963,16 @@
         <v>14</v>
       </c>
       <c r="J8" t="n">
-        <v>1.707089712754549</v>
+        <v>2.478507513310722</v>
       </c>
       <c r="K8" t="n">
-        <v>2.999466478598363</v>
+        <v>0.6973179972408781</v>
       </c>
       <c r="L8" t="n">
-        <v>1.446321398849405</v>
+        <v>1.182006459958566</v>
       </c>
       <c r="M8" t="n">
-        <v>1.780148400507346</v>
+        <v>1.491313139750291</v>
       </c>
       <c r="N8" t="n">
         <v>-31.49879264831543</v>
@@ -1004,16 +1004,16 @@
         <v>44013</v>
       </c>
       <c r="B9" t="n">
-        <v>2.548265390879449</v>
+        <v>-0.5851866069045748</v>
       </c>
       <c r="C9" t="n">
-        <v>5.161811764402577</v>
+        <v>3.859827423951487</v>
       </c>
       <c r="D9" t="n">
-        <v>2.571210205683845</v>
+        <v>1.549208067845804</v>
       </c>
       <c r="E9" t="n">
-        <v>1.924275155794865</v>
+        <v>1.601297700235178</v>
       </c>
       <c r="F9" t="n">
         <v>18.55722618103027</v>
@@ -1028,16 +1028,16 @@
         <v>25.33333396911621</v>
       </c>
       <c r="J9" t="n">
-        <v>2.548265390879449</v>
+        <v>-0.5851866069045748</v>
       </c>
       <c r="K9" t="n">
-        <v>5.161811764402577</v>
+        <v>3.859827423951487</v>
       </c>
       <c r="L9" t="n">
-        <v>2.571210205683845</v>
+        <v>1.549208067845804</v>
       </c>
       <c r="M9" t="n">
-        <v>1.924275155794865</v>
+        <v>1.601297700235178</v>
       </c>
       <c r="N9" t="n">
         <v>18.55722618103027</v>
@@ -1069,16 +1069,16 @@
         <v>44105</v>
       </c>
       <c r="B10" t="n">
-        <v>3.925161465394415</v>
+        <v>1.532569976950621</v>
       </c>
       <c r="C10" t="n">
-        <v>4.573639312412173</v>
+        <v>2.359928885994272</v>
       </c>
       <c r="D10" t="n">
-        <v>2.640929391352556</v>
+        <v>1.930538557116238</v>
       </c>
       <c r="E10" t="n">
-        <v>2.066447829538879</v>
+        <v>1.654336769972793</v>
       </c>
       <c r="F10" t="n">
         <v>14.4931812286377</v>
@@ -1093,16 +1093,16 @@
         <v>9.666666984558105</v>
       </c>
       <c r="J10" t="n">
-        <v>3.925161465394415</v>
+        <v>1.532569976950621</v>
       </c>
       <c r="K10" t="n">
-        <v>4.573639312412173</v>
+        <v>2.359928885994272</v>
       </c>
       <c r="L10" t="n">
-        <v>2.640929391352556</v>
+        <v>1.930538557116238</v>
       </c>
       <c r="M10" t="n">
-        <v>2.066447829538879</v>
+        <v>1.654336769972793</v>
       </c>
       <c r="N10" t="n">
         <v>14.4931812286377</v>
@@ -1134,16 +1134,16 @@
         <v>44197</v>
       </c>
       <c r="B11" t="n">
-        <v>5.41570914763265</v>
+        <v>4.49236174839908</v>
       </c>
       <c r="C11" t="n">
-        <v>8.690423321004072</v>
+        <v>5.619242251286392</v>
       </c>
       <c r="D11" t="n">
-        <v>2.52100251750318</v>
+        <v>2.045174124597719</v>
       </c>
       <c r="E11" t="n">
-        <v>2.160514947755103</v>
+        <v>1.726261054191536</v>
       </c>
       <c r="F11" t="n">
         <v>35.50856399536133</v>
@@ -1158,16 +1158,16 @@
         <v>11.66666698455811</v>
       </c>
       <c r="J11" t="n">
-        <v>5.41570914763265</v>
+        <v>4.49236174839908</v>
       </c>
       <c r="K11" t="n">
-        <v>8.690423321004072</v>
+        <v>5.619242251286392</v>
       </c>
       <c r="L11" t="n">
-        <v>2.52100251750318</v>
+        <v>2.045174124597719</v>
       </c>
       <c r="M11" t="n">
-        <v>2.160514947755103</v>
+        <v>1.726261054191536</v>
       </c>
       <c r="N11" t="n">
         <v>35.50856399536133</v>
@@ -1199,16 +1199,16 @@
         <v>44287</v>
       </c>
       <c r="B12" t="n">
-        <v>4.041327098464382</v>
+        <v>2.426354921777689</v>
       </c>
       <c r="C12" t="n">
-        <v>7.104535720346792</v>
+        <v>6.511403028606294</v>
       </c>
       <c r="D12" t="n">
-        <v>3.246296339093778</v>
+        <v>2.565404917870143</v>
       </c>
       <c r="E12" t="n">
-        <v>2.405517533039561</v>
+        <v>1.883318937686796</v>
       </c>
       <c r="F12" t="n">
         <v>4.392442226409912</v>
@@ -1223,16 +1223,16 @@
         <v>48.33333206176758</v>
       </c>
       <c r="J12" t="n">
-        <v>4.041327098464382</v>
+        <v>2.426354921777689</v>
       </c>
       <c r="K12" t="n">
-        <v>7.104535720346792</v>
+        <v>6.511403028606294</v>
       </c>
       <c r="L12" t="n">
-        <v>3.246296339093778</v>
+        <v>2.565404917870143</v>
       </c>
       <c r="M12" t="n">
-        <v>2.405517533039561</v>
+        <v>1.883318937686796</v>
       </c>
       <c r="N12" t="n">
         <v>4.392442226409912</v>
@@ -1264,16 +1264,16 @@
         <v>44378</v>
       </c>
       <c r="B13" t="n">
-        <v>7.138470407773682</v>
+        <v>3.453365118268367</v>
       </c>
       <c r="C13" t="n">
-        <v>6.223102706575908</v>
+        <v>3.574430157754606</v>
       </c>
       <c r="D13" t="n">
-        <v>3.547903824342392</v>
+        <v>2.617699030388895</v>
       </c>
       <c r="E13" t="n">
-        <v>2.500935234204537</v>
+        <v>1.899968678029008</v>
       </c>
       <c r="F13" t="n">
         <v>17.10367202758789</v>
@@ -1288,16 +1288,16 @@
         <v>22.33333396911621</v>
       </c>
       <c r="J13" t="n">
-        <v>7.138470407773682</v>
+        <v>3.453365118268367</v>
       </c>
       <c r="K13" t="n">
-        <v>6.223102706575908</v>
+        <v>3.574430157754606</v>
       </c>
       <c r="L13" t="n">
-        <v>3.547903824342392</v>
+        <v>2.617699030388895</v>
       </c>
       <c r="M13" t="n">
-        <v>2.500935234204537</v>
+        <v>1.899968678029008</v>
       </c>
       <c r="N13" t="n">
         <v>17.10367202758789</v>
@@ -1329,16 +1329,16 @@
         <v>44470</v>
       </c>
       <c r="B14" t="n">
-        <v>5.88510388946956</v>
+        <v>4.457383385483923</v>
       </c>
       <c r="C14" t="n">
-        <v>8.686755909100066</v>
+        <v>7.812108007885445</v>
       </c>
       <c r="D14" t="n">
-        <v>3.501288734535368</v>
+        <v>2.603983628082156</v>
       </c>
       <c r="E14" t="n">
-        <v>2.657655480666553</v>
+        <v>2.003499679048085</v>
       </c>
       <c r="F14" t="n">
         <v>28.6794490814209</v>
@@ -1353,16 +1353,16 @@
         <v>22</v>
       </c>
       <c r="J14" t="n">
-        <v>5.88510388946956</v>
+        <v>4.457383385483923</v>
       </c>
       <c r="K14" t="n">
-        <v>8.686755909100066</v>
+        <v>7.812108007885445</v>
       </c>
       <c r="L14" t="n">
-        <v>3.501288734535368</v>
+        <v>2.603983628082156</v>
       </c>
       <c r="M14" t="n">
-        <v>2.657655480666553</v>
+        <v>2.003499679048085</v>
       </c>
       <c r="N14" t="n">
         <v>28.6794490814209</v>
@@ -1394,16 +1394,16 @@
         <v>44562</v>
       </c>
       <c r="B15" t="n">
-        <v>5.903278497842052</v>
+        <v>4.741527240123398</v>
       </c>
       <c r="C15" t="n">
-        <v>9.326031465330262</v>
+        <v>8.035795149322816</v>
       </c>
       <c r="D15" t="n">
-        <v>3.788507206940825</v>
+        <v>3.246591233005434</v>
       </c>
       <c r="E15" t="n">
-        <v>2.875771655760958</v>
+        <v>2.200677940063331</v>
       </c>
       <c r="F15" t="n">
         <v>40.09111404418945</v>
@@ -1418,16 +1418,16 @@
         <v>19.66666603088379</v>
       </c>
       <c r="J15" t="n">
-        <v>5.903278497842052</v>
+        <v>4.741527240123398</v>
       </c>
       <c r="K15" t="n">
-        <v>9.326031465330262</v>
+        <v>8.035795149322816</v>
       </c>
       <c r="L15" t="n">
-        <v>3.788507206940825</v>
+        <v>3.246591233005434</v>
       </c>
       <c r="M15" t="n">
-        <v>2.875771655760958</v>
+        <v>2.200677940063331</v>
       </c>
       <c r="N15" t="n">
         <v>40.09111404418945</v>
@@ -1459,16 +1459,16 @@
         <v>44652</v>
       </c>
       <c r="B16" t="n">
-        <v>6.572391498800909</v>
+        <v>4.914510101920945</v>
       </c>
       <c r="C16" t="n">
-        <v>9.855668632346275</v>
+        <v>8.462360184962892</v>
       </c>
       <c r="D16" t="n">
-        <v>4.349832790633939</v>
+        <v>3.518084194922744</v>
       </c>
       <c r="E16" t="n">
-        <v>2.717981976982983</v>
+        <v>2.324739161053456</v>
       </c>
       <c r="F16" t="n">
         <v>30.21818161010742</v>
@@ -1483,16 +1483,16 @@
         <v>32.66666793823242</v>
       </c>
       <c r="J16" t="n">
-        <v>6.572391498800909</v>
+        <v>4.914510101920945</v>
       </c>
       <c r="K16" t="n">
-        <v>9.855668632346275</v>
+        <v>8.462360184962892</v>
       </c>
       <c r="L16" t="n">
-        <v>4.349832790633939</v>
+        <v>3.518084194922744</v>
       </c>
       <c r="M16" t="n">
-        <v>2.717981976982983</v>
+        <v>2.324739161053456</v>
       </c>
       <c r="N16" t="n">
         <v>30.21818161010742</v>
@@ -1524,16 +1524,16 @@
         <v>44743</v>
       </c>
       <c r="B17" t="n">
-        <v>5.231883391341852</v>
+        <v>4.530987644907642</v>
       </c>
       <c r="C17" t="n">
-        <v>1.673691006414161</v>
+        <v>1.086403302456671</v>
       </c>
       <c r="D17" t="n">
-        <v>4.165709660639497</v>
+        <v>3.159679259395985</v>
       </c>
       <c r="E17" t="n">
-        <v>2.591637474714854</v>
+        <v>2.228979836847881</v>
       </c>
       <c r="F17" t="n">
         <v>-46.79662704467773</v>
@@ -1548,16 +1548,16 @@
         <v>18</v>
       </c>
       <c r="J17" t="n">
-        <v>5.231883391341852</v>
+        <v>4.530987644907642</v>
       </c>
       <c r="K17" t="n">
-        <v>1.673691006414161</v>
+        <v>1.086403302456671</v>
       </c>
       <c r="L17" t="n">
-        <v>4.165709660639497</v>
+        <v>3.159679259395985</v>
       </c>
       <c r="M17" t="n">
-        <v>2.591637474714854</v>
+        <v>2.228979836847881</v>
       </c>
       <c r="N17" t="n">
         <v>-46.79662704467773</v>
@@ -1589,16 +1589,16 @@
         <v>44835</v>
       </c>
       <c r="B18" t="n">
-        <v>5.112999863523385</v>
+        <v>4.152352593920312</v>
       </c>
       <c r="C18" t="n">
-        <v>6.10984356365371</v>
+        <v>3.829086583649435</v>
       </c>
       <c r="D18" t="n">
-        <v>3.304065659169891</v>
+        <v>2.308001588488731</v>
       </c>
       <c r="E18" t="n">
-        <v>2.632003991546259</v>
+        <v>2.173252283259402</v>
       </c>
       <c r="F18" t="n">
         <v>-16.02694511413574</v>
@@ -1613,16 +1613,16 @@
         <v>23.66666603088379</v>
       </c>
       <c r="J18" t="n">
-        <v>5.112999863523385</v>
+        <v>4.152352593920312</v>
       </c>
       <c r="K18" t="n">
-        <v>6.10984356365371</v>
+        <v>3.829086583649435</v>
       </c>
       <c r="L18" t="n">
-        <v>3.304065659169891</v>
+        <v>2.308001588488731</v>
       </c>
       <c r="M18" t="n">
-        <v>2.632003991546259</v>
+        <v>2.173252283259402</v>
       </c>
       <c r="N18" t="n">
         <v>-16.02694511413574</v>
@@ -1654,16 +1654,16 @@
         <v>44927</v>
       </c>
       <c r="B19" t="n">
-        <v>5.307787499498914</v>
+        <v>4.17161561064515</v>
       </c>
       <c r="C19" t="n">
-        <v>4.979445338340163</v>
+        <v>3.426370195286472</v>
       </c>
       <c r="D19" t="n">
-        <v>2.790295248693076</v>
+        <v>2.578060717518183</v>
       </c>
       <c r="E19" t="n">
-        <v>2.786496694332275</v>
+        <v>2.255472600394167</v>
       </c>
       <c r="F19" t="n">
         <v>-13.55381965637207</v>
@@ -1678,16 +1678,16 @@
         <v>21.5</v>
       </c>
       <c r="J19" t="n">
-        <v>5.307787499498914</v>
+        <v>4.17161561064515</v>
       </c>
       <c r="K19" t="n">
-        <v>4.979445338340163</v>
+        <v>3.426370195286472</v>
       </c>
       <c r="L19" t="n">
-        <v>2.790295248693076</v>
+        <v>2.578060717518183</v>
       </c>
       <c r="M19" t="n">
-        <v>2.786496694332275</v>
+        <v>2.255472600394167</v>
       </c>
       <c r="N19" t="n">
         <v>-13.55381965637207</v>

</xml_diff>